<commit_message>
Added method to read csv file directly and use it to generate excel excel based report.
</commit_message>
<xml_diff>
--- a/SpringDataR2DBC/src/main/resources/code_review_reports/CodeReviewReport.xlsx
+++ b/SpringDataR2DBC/src/main/resources/code_review_reports/CodeReviewReport.xlsx
@@ -17,16 +17,16 @@
     <t>Project</t>
   </si>
   <si>
-    <t> Version</t>
-  </si>
-  <si>
-    <t> Jira ticket number</t>
+    <t xml:space="preserve"> Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jira ticket number</t>
   </si>
   <si>
     <t>Jira type</t>
   </si>
   <si>
-    <t> Jira ticket summary text</t>
+    <t xml:space="preserve"> Jira ticket summary text</t>
   </si>
   <si>
     <t>Crucible ID</t>
@@ -47,7 +47,7 @@
     <t>Review Date</t>
   </si>
   <si>
-    <t>OPTI</t>
+    <t>"OPTI"</t>
   </si>
   <si>
     <t>OPD - iOS 1.0</t>
@@ -56,10 +56,10 @@
     <t>OPTI-401</t>
   </si>
   <si>
-    <t>Bug</t>
-  </si>
-  <si>
-    <t>Dose display and Dose calculating screen has white background (not consistent)</t>
+    <t>"Bug"</t>
+  </si>
+  <si>
+    <t>"Dose display and Dose calculating screen has white background (not consistent)"</t>
   </si>
   <si>
     <t>Unknown</t>
@@ -83,7 +83,7 @@
     <t>OPTI-394</t>
   </si>
   <si>
-    <t>App crashes, when user tap on 'Record Injected Dose' button, on onboarding day</t>
+    <t>"App crashes</t>
   </si>
   <si>
     <t>Kathleen McGarraugh</t>
@@ -101,7 +101,7 @@
     <t>OPTI-391</t>
   </si>
   <si>
-    <t>User is directly redirected to the dose calculating screen, when they tap on 'Get Dose Recommendation' button on More screen</t>
+    <t>"User is directly redirected to the dose calculating screen</t>
   </si>
   <si>
     <t>OPTI-391 #comment Fixed an issue with incorrectly setting more menu item flags.</t>
@@ -113,7 +113,7 @@
     <t>OPTI-390</t>
   </si>
   <si>
-    <t>User is getting dose confirmation pop up on 'Record Injected dose' flow</t>
+    <t>"User is getting dose confirmation pop up on 'Record Injected dose' flow"</t>
   </si>
   <si>
     <t>OPTI-390 #comment Removed overlay from record injected dose screen.</t>
@@ -125,7 +125,7 @@
     <t>OPTI-387</t>
   </si>
   <si>
-    <t>'FBG Not reported' text is not displaying along with recorded dose, when user record a dose though 'Recorded Injection Dose' flow</t>
+    <t>"'FBG Not reported' text is not displaying along with recorded dose</t>
   </si>
   <si>
     <t>Dustyn August</t>
@@ -143,7 +143,7 @@
     <t>OPTI-386</t>
   </si>
   <si>
-    <t>User cannot edit the dose which user recorded on first day of current dosing window</t>
+    <t>"User cannot edit the dose which user recorded on first day of current dosing window"</t>
   </si>
   <si>
     <t>OPTI-386 #comment reove two day restriction for editing dose</t>
@@ -155,7 +155,7 @@
     <t>OPTI-381</t>
   </si>
   <si>
-    <t>No recommendation dose from icobot when User select a low FBG reading on last 3 days</t>
+    <t>"No recommendation dose from icobot when User select a low FBG reading on last 3 days "</t>
   </si>
   <si>
     <t>OPTI-380, OPTI-381 remove patterns fetching logic</t>
@@ -167,7 +167,7 @@
     <t>OPTI-368</t>
   </si>
   <si>
-    <t>Glooko_2005_013_screenshots_SR-Cyrilic_Opti-33_layout</t>
+    <t>"Glooko_2005_013_screenshots_SR-Cyrilic_Opti-33_layout"</t>
   </si>
   <si>
     <t>Eugene Chiang</t>
@@ -185,7 +185,7 @@
     <t>OPTI-366</t>
   </si>
   <si>
-    <t>'FBG not reported' incorrectly aligned on home screen for insulin days</t>
+    <t>"'FBG not reported' incorrectly aligned on home screen for insulin days"</t>
   </si>
   <si>
     <t>OPTI-366 #comment Updated FBG Not reported to be right aligned.</t>
@@ -197,7 +197,7 @@
     <t>OPTI-360</t>
   </si>
   <si>
-    <t>Dose banner overlaps with the home screen title when displayed and the dose units are displayed below the dose logged text.</t>
+    <t>"Dose banner overlaps with the home screen title when displayed and the dose units are displayed below the dose logged text."</t>
   </si>
   <si>
     <t>OPTI-360 #comment Updated banner.origin.y to nav bar height.</t>
@@ -209,7 +209,7 @@
     <t>OPTI-358</t>
   </si>
   <si>
-    <t>Glooko_2005_013_BG_OPTI-33_Layout</t>
+    <t>" Glooko_2005_013_BG_OPTI-33_Layout"</t>
   </si>
   <si>
     <t>OPTI-354 LOC-344 OPTI-367 OPTI-358 LOC-325 OPTI-356 LOC-333 OPTI-355 LOC-335 OPTI-353 LOC-345 #comment lots of small...</t>
@@ -221,31 +221,31 @@
     <t>OPTI-356</t>
   </si>
   <si>
-    <t>Glooko_2005_013_BG/DE_OPTI-12_Layout of numbered list</t>
+    <t>"Glooko_2005_013_BG/DE_OPTI-12_Layout of numbered list"</t>
   </si>
   <si>
     <t>OPTI-355</t>
   </si>
   <si>
-    <t>ESUS_Glooko_2005_013_Application_OPTI-12_Layout</t>
+    <t>" ESUS_Glooko_2005_013_Application_OPTI-12_Layout"</t>
   </si>
   <si>
     <t>OPTI-354</t>
   </si>
   <si>
-    <t>Glooko_2005_013_DE_OPTI-84_Trunctation</t>
+    <t>" Glooko_2005_013_DE_OPTI-84_Trunctation"</t>
   </si>
   <si>
     <t>OPTI-353</t>
   </si>
   <si>
-    <t>Glooko_2005_013_DE_OPTI-80_Trunctation</t>
+    <t>" Glooko_2005_013_DE_OPTI-80_Trunctation"</t>
   </si>
   <si>
     <t>OPTI-351</t>
   </si>
   <si>
-    <t>Glooko_2005_013_OPTI-16_layout issue</t>
+    <t>" Glooko_2005_013_OPTI-16_layout issue"</t>
   </si>
   <si>
     <t>OPTI-351 LOC-347 #comment fix hungarian space is not actually english space</t>
@@ -257,7 +257,7 @@
     <t>OPTI-346</t>
   </si>
   <si>
-    <t>Glooko_2005_013_OPTI-14_i18n</t>
+    <t>"Glooko_2005_013_OPTI-14_i18n"</t>
   </si>
   <si>
     <t>OPTI-346 LOC-355 #comment deleting extra '.' after 'month' character in hungarian</t>
@@ -269,7 +269,7 @@
     <t>OPTI-342</t>
   </si>
   <si>
-    <t>Glooko_2005_013_TR_OPTI-12_Pair Accu-Chek Guide_layout issue</t>
+    <t>"Glooko_2005_013_TR_OPTI-12_Pair Accu-Chek Guide_layout issue"</t>
   </si>
   <si>
     <t>LOC-365 OPTI-342 #comment temporary language fix for numbered list</t>
@@ -281,7 +281,7 @@
     <t>OPTI-341</t>
   </si>
   <si>
-    <t>Glooko_2005_013_TR_OPTI-12_Layout of numbered list</t>
+    <t>" Glooko_2005_013_TR_OPTI-12_Layout of numbered list"</t>
   </si>
   <si>
     <t>OPTI-341 LOC-366 #comment temporary fix on tutorial instructions</t>
@@ -293,7 +293,7 @@
     <t>OPTI-339</t>
   </si>
   <si>
-    <t>Glooko_2005_013_TR_OPTI-14_i18n_Global</t>
+    <t>"Glooko_2005_013_TR_OPTI-14_i18n_Global"</t>
   </si>
   <si>
     <t>LOC-368 OPTI-339 #comment reformating turkish date format</t>
@@ -305,7 +305,7 @@
     <t>OPTI-336</t>
   </si>
   <si>
-    <t>Nothing happens when user taps on a home screen cell which has dose value </t>
+    <t>"Nothing happens when user taps on a home screen cell which has dose value "</t>
   </si>
   <si>
     <t>OPTI-336 OPTI-324 OPTI-325 OPTI-326 #comment Resolved issues with not being able to edit dose injection. Resolved...</t>
@@ -317,7 +317,7 @@
     <t>OPTI-334</t>
   </si>
   <si>
-    <t>Button text should be 'I Took X Units' for the Record Injection flow</t>
+    <t>"Button text should be 'I Took X Units' for the Record Injection flow"</t>
   </si>
   <si>
     <t>OPTI-334 #comment Updated button to reflect the amount of selected units.</t>
@@ -329,7 +329,7 @@
     <t>OPTI-333</t>
   </si>
   <si>
-    <t>FBG Not Reported is not displaying during first week</t>
+    <t>"FBG Not Reported is not displaying during first week"</t>
   </si>
   <si>
     <t>OPTI-333 #comment Updated canEditFBG to check if date is within two days when no icobot recommendation...</t>
@@ -341,10 +341,10 @@
     <t>OPTI-332</t>
   </si>
   <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>Update restrictions for logging insulin</t>
+    <t>"Task"</t>
+  </si>
+  <si>
+    <t>"Update restrictions for logging insulin"</t>
   </si>
   <si>
     <t>OPTI-332 #comment Change record dose date range and add dialog when attempting to record dose when...</t>
@@ -356,7 +356,7 @@
     <t>OPTI-330</t>
   </si>
   <si>
-    <t>Dose confirmation pop up is displaying on 'I took a different amount' flow</t>
+    <t>"Dose confirmation pop up is displaying on 'I took a different amount' flow"</t>
   </si>
   <si>
     <t>OPTI-330 #comment Removed confirmation overlay from recording dose.</t>
@@ -368,7 +368,7 @@
     <t>OPTI-329</t>
   </si>
   <si>
-    <t>Next injection date is not displaying on Routine screen</t>
+    <t>"Next injection date is not displaying on Routine screen"</t>
   </si>
   <si>
     <t>OPTI-329 #coment Get the next injection day after today if next valid dose day was in the past</t>
@@ -380,7 +380,7 @@
     <t>OPTI-328</t>
   </si>
   <si>
-    <t>Dose value is highlighted when user edits the dose value and recommended dose is expired</t>
+    <t>"Dose value is highlighted when user edits the dose value and recommended dose is expired"</t>
   </si>
   <si>
     <t>OPTI-328 #comment  Added potential fix, to be tested once BE issue is resolved.</t>
@@ -392,13 +392,13 @@
     <t>OPTI-326</t>
   </si>
   <si>
-    <t>Recommended dose is displaying on 'Insulin Dose' screen when User tries to update previous day dose(Recommended dose expired)</t>
+    <t>"Recommended dose is displaying on 'Insulin Dose' screen when User tries to update previous day dose(Recommended dose expired)"</t>
   </si>
   <si>
     <t>OPTI-325</t>
   </si>
   <si>
-    <t>Dose is not displaying on the previous day, after user updates current day dose and select previous day on date selector</t>
+    <t>"Dose is not displaying on the previous day</t>
   </si>
   <si>
     <t>OPTI-325: Dose is not displaying on the previous day, after user updates current day dose and select previous day on date selector</t>
@@ -410,13 +410,13 @@
     <t>OPTI-324</t>
   </si>
   <si>
-    <t>Date selector on the Edit Dose flow can select any day from last 14 days</t>
+    <t>"Date selector on the Edit Dose flow can select any day from last 14 days"</t>
   </si>
   <si>
     <t>OPTI-323</t>
   </si>
   <si>
-    <t>'Dose confirmation' pop up is displaying for 'Edit Dose' flow</t>
+    <t>"'Dose confirmation' pop up is displaying for 'Edit Dose' flow"</t>
   </si>
   <si>
     <t>OPTI-202 OPTI-323 #comment Made changes to the logic, removed overlay.</t>
@@ -428,7 +428,7 @@
     <t>OPTI-322</t>
   </si>
   <si>
-    <t>[Edit Dose]Date information is displaying on 'insulin Dose' screen when the recommended dose is not expired</t>
+    <t>"[Edit Dose]Date information is displaying on 'insulin Dose' screen when the recommended dose is not expired"</t>
   </si>
   <si>
     <t>OPTI-322 #comment Made changes to the layout to reflect design.</t>
@@ -440,7 +440,7 @@
     <t>OPTI-321</t>
   </si>
   <si>
-    <t>Title for Dose confirmation screen is displaying as 'Edit Insulin Dose' instead of 'Insulin Dose'</t>
+    <t>"Title for Dose confirmation screen is displaying as 'Edit Insulin Dose' instead of 'Insulin Dose'"</t>
   </si>
   <si>
     <t>OPTI-321 #comment Fixed title issue.</t>
@@ -452,7 +452,7 @@
     <t>OPTI-318</t>
   </si>
   <si>
-    <t>Delay in displaying the right data on Home screen</t>
+    <t>"Delay in displaying the right data on Home screen"</t>
   </si>
   <si>
     <t>OPTI-318 #comment post notification in main thread</t>
@@ -470,7 +470,7 @@
     <t>OPTI-316</t>
   </si>
   <si>
-    <t>Injection reminder is displayed after suspend by non-adherence /resume even if user went through dose guidance.</t>
+    <t>"Injection reminder is displayed after suspend by non-adherence /resume even if user went through dose guidance."</t>
   </si>
   <si>
     <t>OPTI-316 #comment check for no dose guidance when deciding to skip reminder</t>
@@ -482,7 +482,7 @@
     <t>OPTI-314</t>
   </si>
   <si>
-    <t>Routine screen is not displaying after updating FBG reminder</t>
+    <t>"Routine screen is not displaying after updating FBG reminder"</t>
   </si>
   <si>
     <t>OPTI-314 #comment show routine screen after editing reminder time.</t>
@@ -494,7 +494,7 @@
     <t>OPTI-309</t>
   </si>
   <si>
-    <t>Reminders are not displayed after resume by provider</t>
+    <t>"Reminders are not displayed after resume by provider"</t>
   </si>
   <si>
     <t>OPTI-309 #comment wait for reminder to change before saving context</t>
@@ -506,7 +506,7 @@
     <t>OPTI-307</t>
   </si>
   <si>
-    <t>Various copy updates</t>
+    <t>"Various copy updates"</t>
   </si>
   <si>
     <t>OPTI-307 #comment Updates to various text. Updates to various image assets.</t>
@@ -518,7 +518,7 @@
     <t>OPTI-306</t>
   </si>
   <si>
-    <t>User is not able to add fbg or edit fbg after suspend by non adherence by system/resume </t>
+    <t>"User is not able to add fbg or edit fbg after suspend by non adherence by system/resume "</t>
   </si>
   <si>
     <t>OPTI-169: OPTI-306: Allow user to add FBG if insulin already exists</t>
@@ -530,7 +530,7 @@
     <t>OPTI-303</t>
   </si>
   <si>
-    <t>Suspend by non adherence by system - Dose guide screen is displayed after suspend</t>
+    <t>"Suspend by non adherence by system - Dose guide screen is displayed after suspend"</t>
   </si>
   <si>
     <t>OPTI-303 #comment Added server sync for treatment plan on zero dose guidance.</t>
@@ -542,10 +542,10 @@
     <t>OPTI-301</t>
   </si>
   <si>
-    <t>Improvement</t>
-  </si>
-  <si>
-    <t>Change Optidose to DoseGuide and update app icon</t>
+    <t>"Improvement"</t>
+  </si>
+  <si>
+    <t>"Change Optidose to DoseGuide and update app icon"</t>
   </si>
   <si>
     <t>OPTI-301 #comment Added new app icon. Removed/changed instances of Optidose/Glooko to DoseGuide when...</t>
@@ -557,7 +557,7 @@
     <t>OPTI-299</t>
   </si>
   <si>
-    <t>Suspend for non adherence screen - Phone number is not the same as given in the treatment plan.</t>
+    <t>"Suspend for non adherence screen - Phone number is not the same as given in the treatment plan."</t>
   </si>
   <si>
     <t>OPTI-299 OPTI-295 #comment Updated setTextProperties in GKOptiSuspensionErrorView to set text for...</t>
@@ -569,13 +569,13 @@
     <t>OPTI-295</t>
   </si>
   <si>
-    <t>Investigator name and contact information is not displayed in the suspend screen.</t>
+    <t>"Investigator name and contact information is not displayed in the suspend screen."</t>
   </si>
   <si>
     <t>OPTI-291</t>
   </si>
   <si>
-    <t>User is dropped to home screen when app is killed and reopened half way through onboarding.</t>
+    <t>"User is dropped to home screen when app is killed and reopened half way through onboarding."</t>
   </si>
   <si>
     <t>OPTI-291 #comment Call destroy from on boarding manager to avoid race condition</t>
@@ -593,7 +593,7 @@
     <t>OPTI-289</t>
   </si>
   <si>
-    <t>FBG reminder is displayed for the onboarded day.</t>
+    <t>"FBG reminder is displayed for the onboarded day."</t>
   </si>
   <si>
     <t>OPTI-289 #comment only schedule reminders if start date is a later than today</t>
@@ -605,7 +605,7 @@
     <t>OPTI-288</t>
   </si>
   <si>
-    <t>Hide time for Insulin values</t>
+    <t>"Hide time for Insulin values"</t>
   </si>
   <si>
     <t>OPTI-288 #comment Updated GKReadingInfoView to hide time. Updated GKMedicationHistoryTableViewCell to...</t>
@@ -617,7 +617,7 @@
     <t>OPTI-286</t>
   </si>
   <si>
-    <t>Update logo on splash and loading screen</t>
+    <t>"Update logo on splash and loading screen"</t>
   </si>
   <si>
     <t>OPTI-286 #comment Added Launch Screen, updated logo to new one.</t>
@@ -629,7 +629,7 @@
     <t>OPTI-285</t>
   </si>
   <si>
-    <t>Update prompt to sync if user hasn't synced in last 30 minutes</t>
+    <t>"Update prompt to sync if user hasn't synced in last 30 minutes"</t>
   </si>
   <si>
     <t>OPTI-285 #comment prompt use to sync if they have not for 30 minutes</t>
@@ -641,7 +641,7 @@
     <t>OPTI-284</t>
   </si>
   <si>
-    <t>App crash when user tries to open the app.</t>
+    <t>"App crash when user tries to open the app."</t>
   </si>
   <si>
     <t>OPTI-284 #comment change current dose to baselin dose</t>
@@ -653,7 +653,7 @@
     <t>OPTI-282</t>
   </si>
   <si>
-    <t>New Segment API keys for iOS</t>
+    <t>"New Segment API keys for iOS"</t>
   </si>
   <si>
     <t>OPTI-282 #comment replace segment keys</t>
@@ -665,7 +665,7 @@
     <t>OPTI-279</t>
   </si>
   <si>
-    <t>Baseline dose value is not displaying on confirm dose screen, for Record injection dose flow after the Recommended Dose expiration</t>
+    <t>"Baseline dose value is not displaying on confirm dose screen</t>
   </si>
   <si>
     <t>OPTI-279 #comment Updated parametersForRecordDose() to use baseline dose when no current dose...</t>
@@ -683,7 +683,7 @@
     <t>OPTI-278</t>
   </si>
   <si>
-    <t>Confirmed Insulin Dose value is not displaying on home screen for Record Injection Dose flow</t>
+    <t>"Confirmed Insulin Dose value is not displaying on home screen for Record Injection Dose flow"</t>
   </si>
   <si>
     <t>OPTI-278 #comment Updated fetchData to include the current day.</t>
@@ -695,7 +695,7 @@
     <t>OPTI-275</t>
   </si>
   <si>
-    <t>Remove old pairing if new BGM is paired</t>
+    <t>"Remove old pairing if new BGM is paired"</t>
   </si>
   <si>
     <t>OPTI-275 #comment forget all paired peripherals when going to pair another device</t>
@@ -713,7 +713,7 @@
     <t>OPTI-273</t>
   </si>
   <si>
-    <t>Record injection Dose button is hidden on More screen</t>
+    <t>"Record injection Dose button is hidden on More screen"</t>
   </si>
   <si>
     <t>OPTI-273 #comment Added scroll to top on section change for More menu table view.</t>
@@ -725,7 +725,7 @@
     <t>OPTI-267</t>
   </si>
   <si>
-    <t>Update UI on low bg screen</t>
+    <t>"Update UI on low bg screen"</t>
   </si>
   <si>
     <t>OPTI-267 #comment Updated GKOptiLowBloodGlucoseConfirmationViewController to reflect new design....</t>
@@ -737,7 +737,7 @@
     <t>OPTI-262</t>
   </si>
   <si>
-    <t>Wrong insulin reminder is displaying on injection day when User travels from one timezone to another</t>
+    <t>"Wrong insulin reminder is displaying on injection day when User travels from one timezone to another"</t>
   </si>
   <si>
     <t>OPTI-262 #comment don't compare local and get dates</t>
@@ -749,7 +749,7 @@
     <t>OPTI-256</t>
   </si>
   <si>
-    <t>Lag in displaying Recommended Dose cell to the user</t>
+    <t>"Lag in displaying Recommended Dose cell to the user"</t>
   </si>
   <si>
     <t>OPTI-256 #comment Forcing post for update on all flow ending button taps.</t>
@@ -761,7 +761,7 @@
     <t>OPTI-254</t>
   </si>
   <si>
-    <t>Recommended Dose value is different on Home and Dose display screens</t>
+    <t>"Recommended Dose value is different on Home and Dose display screens"</t>
   </si>
   <si>
     <t>OPTI-254 #comment set the banner's dose value after reuse</t>
@@ -779,7 +779,7 @@
     <t>OPTI-253</t>
   </si>
   <si>
-    <t>User has no option to go back to More screen from BG device list</t>
+    <t>"User has no option to go back to More screen from BG device list"</t>
   </si>
   <si>
     <t>OPTI-253 #comment add cancel button when pairing a new meter</t>
@@ -791,10 +791,10 @@
     <t>OPTI-251</t>
   </si>
   <si>
-    <t>Story</t>
-  </si>
-  <si>
-    <t>Existing user logs in again</t>
+    <t>"Story"</t>
+  </si>
+  <si>
+    <t>"Existing user logs in again"</t>
   </si>
   <si>
     <t>OPTI-251 #comment show data download after paring meter if start adjustment exists</t>
@@ -806,7 +806,7 @@
     <t>OPTI-250</t>
   </si>
   <si>
-    <t>Add Recent FBG Reading pop up is not displaying if user does not have enoughFBG values in last three days</t>
+    <t>"Add Recent FBG Reading pop up is not displaying if user does not have enoughFBG values in last three days"</t>
   </si>
   <si>
     <t>OPTI-250 #comment Date range fix.</t>
@@ -818,7 +818,7 @@
     <t>OPTI-248</t>
   </si>
   <si>
-    <t>Insulin event in the history screen does not have units beside the value</t>
+    <t>"Insulin event in the history screen does not have units beside the value"</t>
   </si>
   <si>
     <t>OPTI-248 #comment assign units to insulin created during dose guidance</t>
@@ -830,7 +830,7 @@
     <t>OPTI-246</t>
   </si>
   <si>
-    <t>Confirmed Insulin dose value is not displaying on home screen for the early injection flow</t>
+    <t>"Confirmed Insulin dose value is not displaying on home screen for the early injection flow"</t>
   </si>
   <si>
     <t>OPTI-246 #comment Added refresh home view notification to deinit of GKOptiGuidanceViewController</t>
@@ -848,7 +848,7 @@
     <t>OPTI-245</t>
   </si>
   <si>
-    <t>QR code error - Invalid error displayed for expired QR code.</t>
+    <t>"QR code error - Invalid error displayed for expired QR code."</t>
   </si>
   <si>
     <t>OPTI-245 #comment Fixed an issue with text copy not being updated prior to displaying error view.</t>
@@ -860,7 +860,7 @@
     <t>OPTI-244</t>
   </si>
   <si>
-    <t>Disable Get Dose Recommendation popup - update OPTI-143</t>
+    <t>"Disable Get Dose Recommendation popup - update OPTI-143"</t>
   </si>
   <si>
     <t>OPTI-244 #comment Added logic to skip guidance overlay as per requirements.</t>
@@ -872,7 +872,7 @@
     <t>OPTI-243</t>
   </si>
   <si>
-    <t>Display banner after dose successfully logged</t>
+    <t>"Display banner after dose successfully logged"</t>
   </si>
   <si>
     <t>OPTI-243 #comment Display a GKNotificationBanner when adding or editing a dose.</t>
@@ -884,7 +884,7 @@
     <t>OPTI-241</t>
   </si>
   <si>
-    <t>End program for participant</t>
+    <t>"End program for participant"</t>
   </si>
   <si>
     <t>OPTI-241 #comment Implemented end program view and logic.</t>
@@ -896,7 +896,7 @@
     <t>OPTI-240</t>
   </si>
   <si>
-    <t>Get Dose recommendaton pop up is not showing if there is not enough FBG reading and user navigates to the dose guidance flow from More screen</t>
+    <t>"Get Dose recommendaton pop up is not showing if there is not enough FBG reading and user navigates to the dose guidance flow from More screen"</t>
   </si>
   <si>
     <t>OPTI-240 #comment Added logic for displaying initial overlay prior to displaying add fbgs overlay.</t>
@@ -908,7 +908,7 @@
     <t>OPTI-238</t>
   </si>
   <si>
-    <t>App crashes when user navigates from More screen to home screen after canceling the dose guidance flow</t>
+    <t>"App crashes when user navigates from More screen to home screen after canceling the dose guidance flow"</t>
   </si>
   <si>
     <t>OPTI-238 #comment Updated layout code so banner is not relative to fbg reading. Updated...</t>
@@ -920,7 +920,7 @@
     <t>OPTI-234</t>
   </si>
   <si>
-    <t>Get Dose recommendation option is displaying after confirming error message on dose display screen</t>
+    <t>"Get Dose recommendation option is displaying after confirming error message on dose display screen"</t>
   </si>
   <si>
     <t>OPTI-234 #comment Fixed issue with label persisting on cell when dose guidance returns zero dose.</t>
@@ -932,7 +932,7 @@
     <t>OPTI-233</t>
   </si>
   <si>
-    <t>Reminders shall make a sound</t>
+    <t>"Reminders shall make a sound"</t>
   </si>
   <si>
     <t>OPTI-233 Added .default sound to UNMutableNotificationContent in...</t>
@@ -944,7 +944,7 @@
     <t>OPTI-232</t>
   </si>
   <si>
-    <t>units is missing for the insulin dose value on home screen</t>
+    <t>"units is missing for the insulin dose value on home screen"</t>
   </si>
   <si>
     <t>OPTI-232 #comment Fixed issue with dose value text.</t>
@@ -956,7 +956,7 @@
     <t>OPTI-231</t>
   </si>
   <si>
-    <t>History - User should not be able to delete or edit Insulin value from history</t>
+    <t>"History - User should not be able to delete or edit Insulin value from history"</t>
   </si>
   <si>
     <t>OPTI-231 #comment remove section and editing handling of history view cells</t>
@@ -968,7 +968,7 @@
     <t>OPTI-229</t>
   </si>
   <si>
-    <t>Unable to proceed from Routine screen</t>
+    <t>"Unable to proceed from Routine screen"</t>
   </si>
   <si>
     <t>OPTI-229 #comment Updates to GKMidsRequestManager</t>
@@ -980,7 +980,7 @@
     <t>OPTI-226</t>
   </si>
   <si>
-    <t>Update hypo threshold in UI to lower limit of target range</t>
+    <t>"Update hypo threshold in UI to lower limit of target range"</t>
   </si>
   <si>
     <t>OPTI-226 #comment Updated isHypo value to the patient's lower limit of their FBG target range.</t>
@@ -992,7 +992,7 @@
     <t>OPTI-224</t>
   </si>
   <si>
-    <t>Pair Accu-Chek Instant</t>
+    <t>"Pair Accu-Chek Instant"</t>
   </si>
   <si>
     <t>OPTI-224 #comment add active flow and tweak pair another meter and log on user flows for Accu chek...</t>
@@ -1010,7 +1010,7 @@
     <t>OPTI-222</t>
   </si>
   <si>
-    <t>Do not ask 'Low BG' question when dose is created or updated by investigator</t>
+    <t>"Do not ask 'Low BG' question when dose is created or updated by investigator"</t>
   </si>
   <si>
     <t>OPTI-222: Do not ask 'Low BG' question when dose is created or updated by investigator</t>
@@ -1022,7 +1022,7 @@
     <t>OPTI-221</t>
   </si>
   <si>
-    <t>Calculating dose screen - When server connection is established again text overlaps calculating dose spinner and error label placeholder is still displayed with no text</t>
+    <t>"Calculating dose screen - When server connection is established again text overlaps calculating dose spinner and error label placeholder is still displayed with no text"</t>
   </si>
   <si>
     <t>OPTI-221 #comment Added logic to block recovery from what is unrecoverable use case.</t>
@@ -1034,7 +1034,7 @@
     <t>OPTI-220</t>
   </si>
   <si>
-    <t>Injection day cell banner is not shown on injection day and also user is not taken to dose guidance flow on injection day</t>
+    <t>"Injection day cell banner is not shown on injection day and also user is not taken to dose guidance flow on injection day"</t>
   </si>
   <si>
     <t>OPTI-220 #comment if previous injection day doesn't exist, use today instead.</t>
@@ -1046,7 +1046,7 @@
     <t>OPTI-218</t>
   </si>
   <si>
-    <t>Localization - Add new country/language [US / Spanish es-US]</t>
+    <t>"Localization - Add new country/language [US / Spanish es-US]"</t>
   </si>
   <si>
     <t>OPTI-218 #comment add logic for spanish language</t>
@@ -1064,7 +1064,7 @@
     <t>OPTI-216</t>
   </si>
   <si>
-    <t>Late injection day cell - Banner for late injection day is not displayed.</t>
+    <t>"Late injection day cell - Banner for late injection day is not displayed."</t>
   </si>
   <si>
     <t>OPTI-216 #comment show late banner when dose guidance is done but dose it not taken that day</t>
@@ -1076,7 +1076,7 @@
     <t>OPTI-215</t>
   </si>
   <si>
-    <t>[Mobile] Add timestamp_utc field to meter Reading collection</t>
+    <t>"[Mobile] Add timestamp_utc field to meter Reading collection"</t>
   </si>
   <si>
     <t>OPTI-215 #comment Added timestampUtc to GKReading/GKMeterSyncReadingParameters</t>
@@ -1088,7 +1088,7 @@
     <t>OPTI-211</t>
   </si>
   <si>
-    <t>Update injection day logic for calendar widget</t>
+    <t>"Update injection day logic for calendar widget"</t>
   </si>
   <si>
     <t>OPTI-211 #comment Updated logic to reflect new requirements.</t>
@@ -1100,7 +1100,7 @@
     <t>OPTI-209</t>
   </si>
   <si>
-    <t>last injection date is displaying as current day on Low Blood Glucose screen</t>
+    <t>"last injection date is displaying as current day on Low Blood Glucose screen"</t>
   </si>
   <si>
     <t>OPTI-209 #comment Updated GKOptiLowBloodGlucoseConfirmationViewController to fetch the most recent...</t>
@@ -1112,7 +1112,7 @@
     <t>OPTI-206</t>
   </si>
   <si>
-    <t>Force data upload prior to dose guidance</t>
+    <t>"Force data upload prior to dose guidance"</t>
   </si>
   <si>
     <t>OPTI-206 #comment check for unsynced objects and sync them before getting dose guidance</t>
@@ -1124,7 +1124,7 @@
     <t>OPTI-205</t>
   </si>
   <si>
-    <t>Suspended for Non-Adherence by System</t>
+    <t>"Suspended for Non-Adherence by System"</t>
   </si>
   <si>
     <t>OPTI-40, OPTI-50, OPTI-205 Suspended by Investigator, Resume by Provider, Suspended for Non-Adherence</t>
@@ -1142,7 +1142,7 @@
     <t>OPTI-202</t>
   </si>
   <si>
-    <t>Edit Dose</t>
+    <t>"Edit Dose"</t>
   </si>
   <si>
     <t>OPTI-202 #comment Added handling for no prior dose guidance case.</t>
@@ -1166,7 +1166,7 @@
     <t>OPTI-194</t>
   </si>
   <si>
-    <t>Localization - Add new country/language [Turkey /Turkish tr-TR]</t>
+    <t>"Localization - Add new country/language [Turkey /Turkish tr-TR]"</t>
   </si>
   <si>
     <t>OPTI-194 #comment Add logic for all new localizations</t>
@@ -1178,7 +1178,7 @@
     <t>OPTI-193</t>
   </si>
   <si>
-    <t>Localization - Add new country/language [Serbia / Serbian sr-Latn-CS ]</t>
+    <t>"Localization - Add new country/language [Serbia / Serbian sr-Latn-CS ]"</t>
   </si>
   <si>
     <t>OPTI-193 #comment Add logic for Serbian localization</t>
@@ -1190,7 +1190,7 @@
     <t>OPTI-192</t>
   </si>
   <si>
-    <t>Manage dose window</t>
+    <t>"Manage dose window"</t>
   </si>
   <si>
     <t>OPTI-192 #comment implement dose availability logic and add tests</t>
@@ -1208,10 +1208,10 @@
     <t>OPTI-191</t>
   </si>
   <si>
-    <t>Technical task</t>
-  </si>
-  <si>
-    <t>Create model for new table cell cases</t>
+    <t>"Technical task"</t>
+  </si>
+  <si>
+    <t>"Create model for new table cell cases"</t>
   </si>
   <si>
     <t>OPTI-191: Create model for new table cell cases</t>
@@ -1229,7 +1229,7 @@
     <t>OPTI-189</t>
   </si>
   <si>
-    <t>Disable and update reminders</t>
+    <t>"Disable and update reminders"</t>
   </si>
   <si>
     <t>OPTI-189 #comment Don't show reminder after user logs FBG or dose</t>
@@ -1241,7 +1241,7 @@
     <t>OPTI-187</t>
   </si>
   <si>
-    <t>Take My Dose from the Home screen</t>
+    <t>"Take My Dose from the Home screen"</t>
   </si>
   <si>
     <t>OPTI-187 #comment Initial push for recommended dose cell.</t>
@@ -1253,7 +1253,7 @@
     <t>OPTI-180</t>
   </si>
   <si>
-    <t>Edit FBG screen - Title should be 'Edit FBG' according to figma</t>
+    <t>"Edit FBG screen - Title should be 'Edit FBG' according to figma"</t>
   </si>
   <si>
     <t>OPTI-180 #comment change label on button and nav bar when editing FBG</t>
@@ -1265,7 +1265,7 @@
     <t>OPTI-174</t>
   </si>
   <si>
-    <t>Confirm FBG screen - Wrong text is displayed on the confirm FBG screen.</t>
+    <t>"Confirm FBG screen - Wrong text is displayed on the confirm FBG screen."</t>
   </si>
   <si>
     <t>OPTI-174 #comment sub in week day if confirming glucose for past day</t>
@@ -1277,7 +1277,7 @@
     <t>OPTI-171</t>
   </si>
   <si>
-    <t>FBG selection screen - BG units are not consistent </t>
+    <t>"FBG selection screen - BG units are not consistent "</t>
   </si>
   <si>
     <t>OPTI-171 #comment fix server sync issues</t>
@@ -1289,13 +1289,13 @@
     <t>OPTI-169</t>
   </si>
   <si>
-    <t>Allow user to add FBG if insulin already exists</t>
+    <t>"Allow user to add FBG if insulin already exists"</t>
   </si>
   <si>
     <t>OPTI-163</t>
   </si>
   <si>
-    <t>FBG explanation screen - User cannot dismiss the screen by tapping outside of the model.</t>
+    <t>"FBG explanation screen - User cannot dismiss the screen by tapping outside of the model."</t>
   </si>
   <si>
     <t>OPTI-163 #comment Updated so view is dismissed when tapping outside of the explanation.</t>
@@ -1307,7 +1307,7 @@
     <t>OPTI-162</t>
   </si>
   <si>
-    <t>UI issue - On the Injection day, FBG icon should be displayed first according to the figma design.</t>
+    <t>"UI issue - On the Injection day</t>
   </si>
   <si>
     <t>OPTI-162 #comment Updated layout to match design.</t>
@@ -1319,7 +1319,7 @@
     <t>OPTI-160</t>
   </si>
   <si>
-    <t>Calender - Injection day does not display the Injection icon.</t>
+    <t>"Calender - Injection day does not display the Injection icon."</t>
   </si>
   <si>
     <t>OPTI-160 #comment Update home screen after setting titration day and fetching treatment plan</t>
@@ -1331,7 +1331,7 @@
     <t>OPTI-155</t>
   </si>
   <si>
-    <t>Display saved insulin value</t>
+    <t>"Display saved insulin value"</t>
   </si>
   <si>
     <t>OPTI-155 #comment save insulin and dismiss dose guidance on confirm dose</t>
@@ -1343,7 +1343,7 @@
     <t>OPTI-151</t>
   </si>
   <si>
-    <t>Various cosmetic updates for design consistency</t>
+    <t>"Various cosmetic updates for design consistency"</t>
   </si>
   <si>
     <t>OPTI-151 #comment Nav bar title text to white.</t>
@@ -1355,7 +1355,7 @@
     <t>OPTI-147</t>
   </si>
   <si>
-    <t>Includes requirement which was not tested as part of OPTI-14</t>
+    <t>"Includes requirement which was not tested as part of OPTI-14"</t>
   </si>
   <si>
     <t>OPTI-147 #comment update range min and max</t>
@@ -1367,7 +1367,7 @@
     <t>OPTI-146</t>
   </si>
   <si>
-    <t>Get dose recommendation Cell</t>
+    <t>"Get dose recommendation Cell"</t>
   </si>
   <si>
     <t>OPTI-146 #comment Remove didSet on isFBGRequirementMet so getDoseButton is always enabled.</t>
@@ -1391,7 +1391,7 @@
     <t>OPTI-145</t>
   </si>
   <si>
-    <t>Prompt to enter FBGs prior to 'Get Dose' on Injection Day</t>
+    <t>"Prompt to enter FBGs prior to 'Get Dose' on Injection Day"</t>
   </si>
   <si>
     <t>OPTI-145 #comment Initial code for a reusable view found in this ticket.</t>
@@ -1409,7 +1409,7 @@
     <t>OPTI-144</t>
   </si>
   <si>
-    <t>Record Injected Dose</t>
+    <t>"Record Injected Dose"</t>
   </si>
   <si>
     <t>OPTI-144 #comment Initial push of GKOptiRecordInjectedDoseViewController and GKOptiDatePicker.</t>
@@ -1427,7 +1427,7 @@
     <t>OPTI-143</t>
   </si>
   <si>
-    <t>Get Dose Recommendation from More</t>
+    <t>"Get Dose Recommendation from More"</t>
   </si>
   <si>
     <t>OPTI-143: Get Dose Recommendation from More</t>
@@ -1439,7 +1439,7 @@
     <t>OPTI-141</t>
   </si>
   <si>
-    <t>I took a different amount</t>
+    <t>"I took a different amount"</t>
   </si>
   <si>
     <t>OPTI-141 #comment Created reusable modal for guidance flow. Added logic for displaying modal when user...</t>
@@ -1451,13 +1451,13 @@
     <t>OPTI-140</t>
   </si>
   <si>
-    <t>UI updates to dose confirmation flow</t>
+    <t>"UI updates to dose confirmation flow"</t>
   </si>
   <si>
     <t>OPTI-138</t>
   </si>
   <si>
-    <t>Calculating dose screen</t>
+    <t>"Calculating dose screen"</t>
   </si>
   <si>
     <t>OPTI-138: Calculating dose screen</t>
@@ -1475,7 +1475,7 @@
     <t>OPTI-137</t>
   </si>
   <si>
-    <t>Low Blood Glucose Screen</t>
+    <t>"Low Blood Glucose Screen"</t>
   </si>
   <si>
     <t>OPTI-137 #comment Initial push for Low Blood Glucose View. Still need to get correct date/day information...</t>
@@ -1487,7 +1487,7 @@
     <t>OPTI-136</t>
   </si>
   <si>
-    <t>Display additional context on FBG screen</t>
+    <t>"Display additional context on FBG screen"</t>
   </si>
   <si>
     <t>OPTI-136 #comment determination header bg color and progress visibility based on the day</t>
@@ -1499,7 +1499,7 @@
     <t>OPTI-135</t>
   </si>
   <si>
-    <t>Cell for late injection day</t>
+    <t>"Cell for late injection day"</t>
   </si>
   <si>
     <t>OPTI-134 OPTI-135 #comment Quick updates from review comments.</t>
@@ -1517,7 +1517,7 @@
     <t>OPTI-134</t>
   </si>
   <si>
-    <t>Injection Day Cell</t>
+    <t>"Injection Day Cell"</t>
   </si>
   <si>
     <t>OPTI-134 #comment Added injection day banner.</t>
@@ -1529,7 +1529,7 @@
     <t>OPTI-132</t>
   </si>
   <si>
-    <t>Includes requirement not tested as part of Edit FBG selection</t>
+    <t>"Includes requirement not tested as part of Edit FBG selection"</t>
   </si>
   <si>
     <t>OPTI-132 #comment Updated didSelectCell to reflect requirements.</t>
@@ -1541,7 +1541,7 @@
     <t>OPTI-125</t>
   </si>
   <si>
-    <t>You are Proconnected pop up displays Glooko instead of dose guide.</t>
+    <t>"You are Proconnected pop up displays Glooko instead of dose guide."</t>
   </si>
   <si>
     <t>OPTI-125 #comment Updated localizable strings to reflect ProConnect designs.</t>
@@ -1553,7 +1553,7 @@
     <t>OPTI-114</t>
   </si>
   <si>
-    <t>Status on the web and server are not updated to InProgress after user successfully on-boards on mobile app.</t>
+    <t>"Status on the web and server are not updated to InProgress after user successfully on-boards on mobile app."</t>
   </si>
   <si>
     <t>OPTI-51 OPTI-114 #comment Changed code to use existing request method for patient adjustments.</t>
@@ -1571,7 +1571,7 @@
     <t>OPTI-113</t>
   </si>
   <si>
-    <t>No error message is displayed when VPN is turned off and user taps on routine screen</t>
+    <t>"No error message is displayed when VPN is turned off and user taps on routine screen"</t>
   </si>
   <si>
     <t>OPTI-113: No error message is displayed when VPN is turned off and user taps on "routine screen"</t>
@@ -1589,7 +1589,7 @@
     <t>OPTI-111</t>
   </si>
   <si>
-    <t>Handle different errors for user log in with participant info</t>
+    <t>"Handle different errors for user log in with participant info"</t>
   </si>
   <si>
     <t>OPTI-111 OPTI-109 OPTI-127 #comment Added error handling display with original designs. Pending changes to logic post...</t>
@@ -1601,7 +1601,7 @@
     <t>OPTI-106</t>
   </si>
   <si>
-    <t>Profile - User is able to add and delete pro connect code.</t>
+    <t>"Profile - User is able to add and delete pro connect code."</t>
   </si>
   <si>
     <t>OPTI-106 #comment Updated table view to not be editable. Removed add button. Updated...</t>
@@ -1613,7 +1613,7 @@
     <t>OPTI-104</t>
   </si>
   <si>
-    <t>Can't scan QR code created via web</t>
+    <t>"Can't scan QR code created via web"</t>
   </si>
   <si>
     <t>OPTI-104 #comment Updated GKScannerViewController.onSuccess() to push next view controller on main...</t>
@@ -1625,7 +1625,7 @@
     <t>OPTI-102</t>
   </si>
   <si>
-    <t>User does not land on home screen when tapped on reminder notification</t>
+    <t>"User does not land on home screen when tapped on reminder notification"</t>
   </si>
   <si>
     <t>OPTI-102 #comment Show home screen when opening from reminder after wreath if necessary</t>
@@ -1637,7 +1637,7 @@
     <t>OPTI-99</t>
   </si>
   <si>
-    <t>Prompt user to sync</t>
+    <t>"Prompt user to sync"</t>
   </si>
   <si>
     <t>OPTI-99 #comment Show sync prompt when user tries to select FBG without syncing</t>
@@ -1649,7 +1649,7 @@
     <t>OPTI-98</t>
   </si>
   <si>
-    <t>Home screen empty state</t>
+    <t>"Home screen empty state"</t>
   </si>
   <si>
     <t>OPTI-98 #comment Updated GKOptiHomeViewController to reflect enpty state for onboarding day.</t>
@@ -1661,7 +1661,7 @@
     <t>OPTI-97</t>
   </si>
   <si>
-    <t>Multiple reminders are displayed for the non injection day.</t>
+    <t>"Multiple reminders are displayed for the non injection day."</t>
   </si>
   <si>
     <t>Dominik Babic,Michael Bader</t>
@@ -1676,7 +1676,7 @@
     <t>OPTI-94</t>
   </si>
   <si>
-    <t>Edit FBG selection</t>
+    <t>"Edit FBG selection"</t>
   </si>
   <si>
     <t>OPTI-94 #comment provide existing FBGs and edit the FBG if user changes</t>
@@ -1688,7 +1688,7 @@
     <t>OPTI-88</t>
   </si>
   <si>
-    <t>Home screen list view</t>
+    <t>"Home screen list view"</t>
   </si>
   <si>
     <t>Dora Fundak,Kathleen McGarraugh,Dustyn August</t>
@@ -1739,7 +1739,7 @@
     <t>OPTI-87</t>
   </si>
   <si>
-    <t>FBG Explanation Screen</t>
+    <t>"FBG Explanation Screen"</t>
   </si>
   <si>
     <t>OPTI-87 #comment Added fbg explanation that is displayed when clicked on information button.</t>
@@ -1751,7 +1751,7 @@
     <t>OPTI-86</t>
   </si>
   <si>
-    <t>FBG Selection Screen</t>
+    <t>"FBG Selection Screen"</t>
   </si>
   <si>
     <t>OPTI-86: FBG Selection Screen</t>
@@ -1769,7 +1769,7 @@
     <t>OPTI-85</t>
   </si>
   <si>
-    <t>Display cell with multiple entries</t>
+    <t>"Display cell with multiple entries"</t>
   </si>
   <si>
     <t>OPTI-82 OPTI-85 #comment Updated cell to support add fbg, single/multiple values, and missed FBG....</t>
@@ -1781,7 +1781,7 @@
     <t>OPTI-84</t>
   </si>
   <si>
-    <t>Calendar widget</t>
+    <t>"Calendar widget"</t>
   </si>
   <si>
     <t>OPTI-84 #comment Added logic for populating and displaying cells of calendar widget. Added logic for...</t>
@@ -1793,13 +1793,13 @@
     <t>OPTI-82</t>
   </si>
   <si>
-    <t>Display cells with a single value</t>
+    <t>"Display cells with a single value"</t>
   </si>
   <si>
     <t>OPTI-80</t>
   </si>
   <si>
-    <t>Cell to Add FBG</t>
+    <t>"Cell to Add FBG"</t>
   </si>
   <si>
     <t>OPTI-80 #comment Added initial table view cell for adding fbg.</t>
@@ -1811,7 +1811,7 @@
     <t>OPTI-77</t>
   </si>
   <si>
-    <t>Pair Accu-Chek Guide tutorial screen should have a back button.</t>
+    <t>"Pair Accu-Chek Guide tutorial screen should have a back button."</t>
   </si>
   <si>
     <t>OPTI-77 #comment Added a back button that takes user back the to the BG Meter selection screen.</t>
@@ -1829,7 +1829,7 @@
     <t>OPTI-73</t>
   </si>
   <si>
-    <t>Pair another BGM</t>
+    <t>"Pair another BGM"</t>
   </si>
   <si>
     <t>OPTI-73 #comment add option to pair another bg meter from More</t>
@@ -1841,7 +1841,7 @@
     <t>OPTI-67</t>
   </si>
   <si>
-    <t>Update Injection Day UI and Routine Screen</t>
+    <t>"Update Injection Day UI and Routine Screen"</t>
   </si>
   <si>
     <t>OPTI-67 #comment Update injection day and routine screens and show routine screen on editing injection...</t>
@@ -1853,7 +1853,7 @@
     <t>OPTI-65</t>
   </si>
   <si>
-    <t>Accu check guide - Button on the first page of the tutorial should be Start</t>
+    <t>"Accu check guide - Button on the first page of the tutorial should be Start"</t>
   </si>
   <si>
     <t>Dora Fundak,Dominik Babic</t>
@@ -1868,7 +1868,7 @@
     <t>OPTI-64</t>
   </si>
   <si>
-    <t>In the Daily reminder FBG screen - Fasting Blood Glucose text should be in Bold text</t>
+    <t>"In the Daily reminder FBG screen - Fasting Blood Glucose text should be in Bold text"</t>
   </si>
   <si>
     <t>OPTI-64: In the "Daily reminder FBG" screen - "Fasting Blood Glucose" text should be in Bold text</t>
@@ -1880,7 +1880,7 @@
     <t>OPTI-63</t>
   </si>
   <si>
-    <t>Create Patient Details Confirmation View</t>
+    <t>"Create Patient Details Confirmation View"</t>
   </si>
   <si>
     <t>OPTI-63 #comment Update tappedYesButton() functionality. Updated unit tests.</t>
@@ -1910,7 +1910,7 @@
     <t>OPTI-62</t>
   </si>
   <si>
-    <t>Create Scan QR Splash Screen</t>
+    <t>"Create Scan QR Splash Screen"</t>
   </si>
   <si>
     <t>OPTI-62 #comment Created initial UI for Scan QR splash. Added placeholder image and localized strings...</t>
@@ -1928,7 +1928,7 @@
     <t>OPTI-61</t>
   </si>
   <si>
-    <t>User not able to login to Dose guide app</t>
+    <t>"User not able to login to Dose guide app"</t>
   </si>
   <si>
     <t>OPTI-61 #comment fix fallback US url</t>
@@ -1940,7 +1940,7 @@
     <t>OPTI-60</t>
   </si>
   <si>
-    <t>Create Touch ID Splash View</t>
+    <t>"Create Touch ID Splash View"</t>
   </si>
   <si>
     <t>OPTI-60 #comment Created initial UI for TouchID splash screen. Added placeholder images and localized...</t>
@@ -1958,7 +1958,7 @@
     <t>OPTI-51</t>
   </si>
   <si>
-    <t>Update patient status to 'Active'</t>
+    <t>"Update patient status to 'Active'"</t>
   </si>
   <si>
     <t>OPTI-51 #comment Model update, commented out code related to removed properties. Added button to home...</t>
@@ -1970,13 +1970,13 @@
     <t>OPTI-50</t>
   </si>
   <si>
-    <t>Resume by Provider</t>
+    <t>"Resume by Provider"</t>
   </si>
   <si>
     <t>OPTI-49</t>
   </si>
   <si>
-    <t>Change Injection Day</t>
+    <t>"Change Injection Day"</t>
   </si>
   <si>
     <t>OPTI-49: Change Injection Day</t>
@@ -1988,7 +1988,7 @@
     <t>OPTI-48</t>
   </si>
   <si>
-    <t>View Help</t>
+    <t>"View Help"</t>
   </si>
   <si>
     <t>OPTI-48 #comment Implemented Help controller.</t>
@@ -2000,7 +2000,7 @@
     <t>OPTI-46</t>
   </si>
   <si>
-    <t>View About</t>
+    <t>"View About"</t>
   </si>
   <si>
     <t>OPTI-46 #comment Implemented About view controller.</t>
@@ -2018,7 +2018,7 @@
     <t>OPTI-43</t>
   </si>
   <si>
-    <t>User able to enter food and other events when tapped on BG reading.</t>
+    <t>"User able to enter food and other events when tapped on BG reading."</t>
   </si>
   <si>
     <t>Michael Bader</t>
@@ -2033,7 +2033,7 @@
     <t>OPTI-41</t>
   </si>
   <si>
-    <t>Display landing page on first time use</t>
+    <t>"Display landing page on first time use"</t>
   </si>
   <si>
     <t>OPTI-41 #comment Created landing page that starts onboarding flow. TODO: Add corrent image and label...</t>
@@ -2051,13 +2051,13 @@
     <t>OPTI-40</t>
   </si>
   <si>
-    <t>Suspended by Investigator</t>
+    <t>"Suspended by Investigator"</t>
   </si>
   <si>
     <t>OPTI-38</t>
   </si>
   <si>
-    <t>UI- More tab &gt; There is a small image beside Profile Name which is not mentioned in the design.</t>
+    <t>"UI- More tab &gt; There is a small image beside Profile Name which is not mentioned in the design."</t>
   </si>
   <si>
     <t>OPTI-38 #comment remove profile image</t>
@@ -2081,7 +2081,7 @@
     <t>OPTI-37</t>
   </si>
   <si>
-    <t>Create reminder time UI</t>
+    <t>"Create reminder time UI"</t>
   </si>
   <si>
     <t>Dora Fundak</t>
@@ -2102,7 +2102,7 @@
     <t>OPTI-36</t>
   </si>
   <si>
-    <t>View Profile</t>
+    <t>"View Profile"</t>
   </si>
   <si>
     <t>OPTI-36 #comment Updated profile page to reflect new design. Added some unit tests</t>
@@ -2126,7 +2126,7 @@
     <t>OPTI-35</t>
   </si>
   <si>
-    <t>Change colors of tab bar</t>
+    <t>"Change colors of tab bar"</t>
   </si>
   <si>
     <t>OPTI-35 #comment Change tab bar icons and update tab bar background</t>
@@ -2138,16 +2138,16 @@
     <t>OPTI-34</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>View More menu</t>
+    <t>"Test"</t>
+  </si>
+  <si>
+    <t>"View More menu"</t>
   </si>
   <si>
     <t>OPTI-33</t>
   </si>
   <si>
-    <t>Configure Touch ID</t>
+    <t>"Configure Touch ID"</t>
   </si>
   <si>
     <t>OPTI-33: Configure Touch ID</t>
@@ -2159,13 +2159,13 @@
     <t>OPTI-32</t>
   </si>
   <si>
-    <t>Home screen should be renamed to Optidose</t>
+    <t>"Home screen should be renamed to Optidose"</t>
   </si>
   <si>
     <t>OPTI-31</t>
   </si>
   <si>
-    <t>Change reminder time</t>
+    <t>"Change reminder time"</t>
   </si>
   <si>
     <t>OPTI-31 #comment Add new FBG screen to more menu</t>
@@ -2177,7 +2177,7 @@
     <t>OPTI-30</t>
   </si>
   <si>
-    <t>The app shall have a tab bar for navigation</t>
+    <t>"The app shall have a tab bar for navigation"</t>
   </si>
   <si>
     <t>OPTI-300 #comment Fixed crash when attempting to show mids flow after sync.</t>
@@ -2189,7 +2189,7 @@
     <t>OPTI-29</t>
   </si>
   <si>
-    <t>Deliver reminders to patient to check FBG</t>
+    <t>"Deliver reminders to patient to check FBG"</t>
   </si>
   <si>
     <t>OPTI-29 #comment adjust reminders to send different message depending on injection day</t>
@@ -2201,7 +2201,7 @@
     <t>OPTI-27</t>
   </si>
   <si>
-    <t>Require Touch ID/passcode to use app</t>
+    <t>"Require Touch ID/passcode to use app"</t>
   </si>
   <si>
     <t>OPTI-27: Require Touch ID/passcode to use app</t>
@@ -2219,7 +2219,7 @@
     <t>OPTI-26</t>
   </si>
   <si>
-    <t>Confirm patient details</t>
+    <t>"Confirm patient details"</t>
   </si>
   <si>
     <t>OPTI-26 Updated GKUser for yearOfBirth. GKQRScannerViewController pushes to details confirmation...</t>
@@ -2231,7 +2231,7 @@
     <t>OPTI-25</t>
   </si>
   <si>
-    <t>Scan QR Code</t>
+    <t>"Scan QR Code"</t>
   </si>
   <si>
     <t>OPTI-25 #comment Updated logic for GKOptiLoginManager, updated unit tests.</t>
@@ -2261,7 +2261,7 @@
     <t>OPTI-23</t>
   </si>
   <si>
-    <t>Remove anything but insulin, BG, and notes from history list</t>
+    <t>"Remove anything but insulin</t>
   </si>
   <si>
     <t>OPTI-23 #comment remove server sync for unused classes.  Remove logic for display in history list</t>
@@ -2276,7 +2276,7 @@
     <t>OPTI-21</t>
   </si>
   <si>
-    <t>Select meter</t>
+    <t>"Select meter"</t>
   </si>
   <si>
     <t>OPTI-21 #comment Update meter list to just show two accu check devices and show at beginning of on...</t>
@@ -2288,7 +2288,7 @@
     <t>OPTI-19</t>
   </si>
   <si>
-    <t>Set Reminder Time</t>
+    <t>"Set Reminder Time"</t>
   </si>
   <si>
     <t>OPTI-19 #comment Add reminder time to on boarding flow and update the reminder time</t>
@@ -2300,13 +2300,13 @@
     <t>OPTI-18</t>
   </si>
   <si>
-    <t>Display next steps screen to the user</t>
+    <t>"Display next steps screen to the user"</t>
   </si>
   <si>
     <t>OPTI-17</t>
   </si>
   <si>
-    <t>Remove meal tags</t>
+    <t>"Remove meal tags"</t>
   </si>
   <si>
     <t>OPTI-17 #comment remove meal tags from readings cell</t>
@@ -2318,7 +2318,7 @@
     <t>OPTI-16</t>
   </si>
   <si>
-    <t>View Home screen</t>
+    <t>"View Home screen"</t>
   </si>
   <si>
     <t>OPTI-16: View Home screen</t>
@@ -2345,7 +2345,7 @@
     <t>OPTI-13</t>
   </si>
   <si>
-    <t>Set Injection Day</t>
+    <t>"Set Injection Day"</t>
   </si>
   <si>
     <t>OPTI-13 #comment set injection day when leaving injection day page</t>
@@ -2381,7 +2381,7 @@
     <t>OPTI-12</t>
   </si>
   <si>
-    <t>Pair Accu-Chek Guide</t>
+    <t>"Pair Accu-Chek Guide"</t>
   </si>
   <si>
     <t>OPTI-12 #comment rename Parent tutorial view controller</t>
@@ -2429,19 +2429,19 @@
     <t>OPTI-9</t>
   </si>
   <si>
-    <t>Create new app center and bitrise builds</t>
+    <t>"Create new app center and bitrise builds"</t>
   </si>
   <si>
     <t>OPTI-8</t>
   </si>
   <si>
-    <t>Create new app id, certificates and provisioning profile</t>
+    <t>"Create new app id</t>
   </si>
   <si>
     <t>OPTI-7</t>
   </si>
   <si>
-    <t>Rename app, bundle id, and remove additional targets</t>
+    <t>"Rename app</t>
   </si>
   <si>
     <t>OPTI-7: Rename app, bundle id, and remove additional targets</t>
@@ -2453,13 +2453,13 @@
     <t>OPTI-6</t>
   </si>
   <si>
-    <t>Glooko Lite POC</t>
+    <t>"Glooko Lite POC"</t>
   </si>
   <si>
     <t>OPTI-5</t>
   </si>
   <si>
-    <t>Remove unused code from app</t>
+    <t>"Remove unused code from app"</t>
   </si>
   <si>
     <t>OPTI-52 #comment UI for Routine screen</t>
@@ -2477,7 +2477,7 @@
     <t>OPTI-4</t>
   </si>
   <si>
-    <t>Remove Add Event Button from Tab bar</t>
+    <t>"Remove Add Event Button from Tab bar"</t>
   </si>
   <si>
     <t>OPTI-44 #comment Added logic for displaying meal tag.</t>
@@ -2489,7 +2489,7 @@
     <t>OPTI-3</t>
   </si>
   <si>
-    <t>Remove Graphs History List</t>
+    <t>"Remove Graphs History List"</t>
   </si>
   <si>
     <t>OPTI-3: Remove Graphs History List</t>
@@ -2519,7 +2519,7 @@
     <t>OPTI-2</t>
   </si>
   <si>
-    <t>Remove Graphs Tab</t>
+    <t>"Remove Graphs Tab"</t>
   </si>
   <si>
     <t>OPTI-2: Remove Graphs Tab</t>
@@ -2537,7 +2537,7 @@
     <t>OPTI-1</t>
   </si>
   <si>
-    <t>Remove unused options from More Menu and Profile</t>
+    <t>"Remove unused options from More Menu and Profile"</t>
   </si>
   <si>
     <t>OPTI-1 #comment remove unused files</t>

</xml_diff>